<commit_message>
Reach Ranks - corrected so all confinement scores pulled
</commit_message>
<xml_diff>
--- a/Output/Spring_Chinook_Ranks_ALL_OUTPUT_Methow_Entiat_Wenatchee_Okanogan.xlsx
+++ b/Output/Spring_Chinook_Ranks_ALL_OUTPUT_Methow_Entiat_Wenatchee_Okanogan.xlsx
@@ -4251,7 +4251,7 @@
       </c>
       <c r="I75" t="inlineStr">
         <is>
-          <t>Coarse Substrate,Cover- Wood,Off-Channel- Floodplain,Coarse Substrate,Cover- Undercut Banks,Cover- Wood,Flow- Summer Base Flow,Off-Channel- Floodplain,Pool Quantity &amp; Quality,% Fines/Embeddedness,Coarse Substrate,Cover- Wood,Off-Channel- Floodplain</t>
+          <t>No Priority Life Stages with Limiting Factors</t>
         </is>
       </c>
       <c r="J75" t="inlineStr">
@@ -4261,7 +4261,7 @@
       </c>
       <c r="K75" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="L75">
@@ -10041,11 +10041,6 @@
           <t>Winter Rearing</t>
         </is>
       </c>
-      <c r="I177" t="inlineStr">
-        <is>
-          <t>No Priority Life Stages with Limiting Factors</t>
-        </is>
-      </c>
       <c r="J177" t="inlineStr">
         <is>
           <t>yes</t>
@@ -10053,7 +10048,7 @@
       </c>
       <c r="K177" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="L177">
@@ -20462,11 +20457,6 @@
       <c r="G373">
         <v>0.4666666666666667</v>
       </c>
-      <c r="I373" t="inlineStr">
-        <is>
-          <t>No Priority Life Stages with Limiting Factors</t>
-        </is>
-      </c>
       <c r="J373" t="inlineStr">
         <is>
           <t>yes</t>
@@ -20474,7 +20464,7 @@
       </c>
       <c r="K373" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="L373">
@@ -21260,11 +21250,6 @@
       <c r="G387">
         <v>0.4222222222222222</v>
       </c>
-      <c r="I387" t="inlineStr">
-        <is>
-          <t>No Priority Life Stages with Limiting Factors</t>
-        </is>
-      </c>
       <c r="J387" t="inlineStr">
         <is>
           <t>yes</t>
@@ -21272,7 +21257,7 @@
       </c>
       <c r="K387" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="L387">
@@ -33880,7 +33865,7 @@
       </c>
       <c r="I649" t="inlineStr">
         <is>
-          <t>Cover- Wood,Off-Channel- Floodplain,Off-Channel- Side-Channels</t>
+          <t>No Priority Life Stages with Limiting Factors</t>
         </is>
       </c>
       <c r="J649" t="inlineStr">
@@ -33890,7 +33875,7 @@
       </c>
       <c r="K649" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="L649">
@@ -34713,7 +34698,7 @@
       </c>
       <c r="I663" t="inlineStr">
         <is>
-          <t>Cover- Wood,Off-Channel- Floodplain,Off-Channel- Side-Channels</t>
+          <t>No Priority Life Stages with Limiting Factors</t>
         </is>
       </c>
       <c r="J663" t="inlineStr">
@@ -34723,7 +34708,7 @@
       </c>
       <c r="K663" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="L663">

</xml_diff>